<commit_message>
add some try catch when creating, reading file
</commit_message>
<xml_diff>
--- a/test_sheets.xlsx
+++ b/test_sheets.xlsx
@@ -5,17 +5,33 @@
   <x:workbookPr defaultThemeVersion="166925"/>
   <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Csharp\excelExport\"/>
   <x:bookViews>
-    <x:workbookView xWindow="1125" yWindow="1110" windowWidth="14850" windowHeight="10560"/>
+    <x:workbookView xWindow="1125" yWindow="1110" windowWidth="14850" windowHeight="10560" activeTab="1"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="mySheet" sheetId="1" r:id="rId1"/>
-    <x:sheet name="mynewsheet" sheetId="2" r:id="Rca62f80961cf4a2d"/>
-    <x:sheet name="mynewsheet2" sheetId="3" r:id="R3cd0c6c37ce04e90"/>
-    <x:sheet name="mynewsheet3" sheetId="4" r:id="R09557a1e85c2447d"/>
+    <x:sheet name="mynewsheet" sheetId="2" r:id="rId2"/>
+    <x:sheet name="mynewsheet2" sheetId="3" r:id="rId3"/>
+    <x:sheet name="mynewsheet3" sheetId="4" r:id="rId4"/>
+    <x:sheet name="mynewsheet1231" sheetId="5" r:id="R611fcc7a7f554620"/>
+    <x:sheet name="Sheet5" sheetId="6" r:id="R28934dd3f5034d32"/>
+    <x:sheet name="Sheet6" sheetId="7" r:id="R15a6886db570424c"/>
   </x:sheets>
   <x:calcPr calcId="0"/>
-  <x:fileRecoveryPr repairLoad="1"/>
 </x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <x:si>
+    <x:t>sdfasf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sassdasasdasd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>asdasd</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -856,7 +872,7 @@
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac xr xr2 xr3">
   <x:dimension ref="A1:B9"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
@@ -879,20 +895,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetData/>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetData/>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetData/>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </x:worksheet>
 </file>
 
@@ -900,4 +952,28 @@
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetData/>
+</x:worksheet>
 </file>
</xml_diff>